<commit_message>
Agregadas las palabras nuevas al código y actualizado el Excel
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\TP final\TP final php\wordix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B7256C-7FB6-4A85-8BFE-5A046D70FD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD19E17A-AD5E-4DE6-BE5E-4C556C7619F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
-    <sheet name="EstructurasDeWordix.php" sheetId="2" r:id="rId2"/>
+    <sheet name="programa" sheetId="1" r:id="rId1"/>
+    <sheet name="wordix.php" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -75,9 +75,6 @@
     <t>¿Para qué se utilizada?: guarda las palabras que se pueden utilizar para jugar wordix</t>
   </si>
   <si>
-    <t>**** SEGUIR COMPLETANDO ****</t>
-  </si>
-  <si>
     <t>//claves</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Pedro</t>
   </si>
   <si>
-    <t>Sol</t>
-  </si>
-  <si>
     <t>¿Para qué es utilizada?: Guarda información de las distintas partidas que se jugaron.</t>
   </si>
   <si>
@@ -213,21 +207,6 @@
     <t>¿Para qué es utilizada?:  Genera un teclado en pantalla en el orden correcto.</t>
   </si>
   <si>
-    <t>$estructuraIntentosWordix=</t>
-  </si>
-  <si>
-    <t>Tipo:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipos de datos: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Para qué es utilizada?: </t>
-  </si>
-  <si>
-    <t>linea 211 de wordix.php</t>
-  </si>
-  <si>
     <t>linea 187 de wordix.php</t>
   </si>
   <si>
@@ -237,9 +216,6 @@
     <t>(se actualiza con función de la línea 280)</t>
   </si>
   <si>
-    <t>(se actualiza con función de la línea 246)</t>
-  </si>
-  <si>
     <t>$estructuraPalabraIntento=</t>
   </si>
   <si>
@@ -270,22 +246,52 @@
     <t>linea 301 de wordix.php</t>
   </si>
   <si>
-    <t>$partida=</t>
-  </si>
-  <si>
-    <t>"QUESO"</t>
-  </si>
-  <si>
-    <t>Tipo: Asociativo (las claves son strings)</t>
-  </si>
-  <si>
-    <t>¿Para qué es utilizada?:  Se utiliza para resumir una partida para usarla luego en estadísticas; cada uno de estos arreglos después va en $coleccionPartidas.</t>
-  </si>
-  <si>
     <t>¿Para qué es utilizada?: Guarda información sobre un cierto jugador, se va a ejecutar solo cuando el jugador pida el resumen y se llena con los datos de $coleccionPartidas.</t>
   </si>
   <si>
     <t>punto c)</t>
+  </si>
+  <si>
+    <t>GOTAS</t>
+  </si>
+  <si>
+    <t>HUEVO</t>
+  </si>
+  <si>
+    <t>TINTO</t>
+  </si>
+  <si>
+    <t>NAVES</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
+    <t>MELON</t>
+  </si>
+  <si>
+    <t>YUYOS</t>
+  </si>
+  <si>
+    <t>PIANO</t>
+  </si>
+  <si>
+    <t>PISOS</t>
+  </si>
+  <si>
+    <t>ACERO</t>
+  </si>
+  <si>
+    <t>BALDE</t>
+  </si>
+  <si>
+    <t>TAZAS</t>
+  </si>
+  <si>
+    <t>JAULA</t>
+  </si>
+  <si>
+    <t>ZORRO</t>
   </si>
 </sst>
 </file>
@@ -435,15 +441,19 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -480,14 +490,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P1000"/>
+  <dimension ref="A3:V1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:H53"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -714,11 +730,11 @@
     <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="26" width="10.7109375" customWidth="1"/>
+    <col min="9" max="21" width="26" customWidth="1"/>
+    <col min="22" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,11 +756,53 @@
       <c r="G3" s="2">
         <v>5</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="2">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2">
+        <v>9</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2">
+        <v>12</v>
+      </c>
+      <c r="O3" s="2">
+        <v>13</v>
+      </c>
+      <c r="P3" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>15</v>
+      </c>
+      <c r="R3" s="2">
+        <v>16</v>
+      </c>
+      <c r="S3" s="2">
+        <v>17</v>
+      </c>
+      <c r="T3" s="2">
+        <v>18</v>
+      </c>
+      <c r="U3" s="2">
+        <v>19</v>
+      </c>
+      <c r="V3" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -760,100 +818,207 @@
       <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q4" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="S4" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="U4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="V4" s="20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2">
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5">
+        <v>3</v>
+      </c>
+      <c r="F15" s="5">
+        <v>4</v>
+      </c>
+      <c r="G15" s="5">
+        <v>5</v>
+      </c>
+      <c r="H15" s="5">
+        <v>6</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5">
+        <v>4</v>
+      </c>
+      <c r="F16" s="5">
+        <v>3</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2</v>
+      </c>
+      <c r="H16" s="5">
         <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="F15" s="2">
-        <v>3</v>
-      </c>
-      <c r="G15" s="2">
-        <v>4</v>
-      </c>
-      <c r="H15" s="2">
-        <v>5</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>8</v>
@@ -863,242 +1028,167 @@
       <c r="P16" s="7"/>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>8</v>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5">
-        <v>2</v>
-      </c>
-      <c r="E18" s="5">
-        <v>3</v>
-      </c>
-      <c r="F18" s="5">
-        <v>4</v>
-      </c>
-      <c r="G18" s="5">
-        <v>5</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="L18" s="6"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="5">
-        <v>6</v>
-      </c>
-      <c r="D19" s="5">
-        <v>5</v>
-      </c>
-      <c r="E19" s="5">
-        <v>4</v>
-      </c>
-      <c r="F19" s="5">
-        <v>3</v>
-      </c>
-      <c r="G19" s="5">
-        <v>2</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>8</v>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="8"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L21" s="6"/>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="9">
+        <v>3</v>
+      </c>
+      <c r="D26" s="10">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E26" s="9">
+        <v>2</v>
+      </c>
+      <c r="F26" s="9">
+        <v>1</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0</v>
+      </c>
+      <c r="K26" s="5">
+        <v>1</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="B28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="9">
-        <v>15</v>
-      </c>
-      <c r="D29" s="10">
-        <v>123</v>
-      </c>
-      <c r="E29" s="9">
-        <v>10</v>
-      </c>
-      <c r="F29" s="9">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9">
-        <v>0</v>
-      </c>
-      <c r="H29" s="10">
-        <v>1</v>
-      </c>
-      <c r="I29" s="10">
-        <v>1</v>
-      </c>
-      <c r="J29" s="5">
-        <v>5</v>
-      </c>
-      <c r="K29" s="5">
-        <v>2</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B31" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1134,10 +1224,10 @@
     <row r="81" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D83" s="18"/>
+      <c r="D83" s="17"/>
     </row>
     <row r="84" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C84" s="18"/>
+      <c r="C84" s="17"/>
     </row>
     <row r="85" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2064,404 +2154,323 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6BA7D5C-A544-4A79-97A4-81E2544FB561}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A2:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="I2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="12"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="B5" s="12"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>21</v>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>66</v>
-      </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="H7" s="8"/>
+      <c r="E7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
+      <c r="B9" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12">
+        <v>2</v>
+      </c>
+      <c r="E11" s="12">
+        <v>3</v>
+      </c>
+      <c r="F11" s="12">
+        <v>4</v>
+      </c>
+      <c r="G11" s="12">
+        <v>5</v>
+      </c>
+      <c r="H11" s="12">
+        <v>6</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="12">
-        <v>0</v>
-      </c>
-      <c r="C10" s="12">
-        <v>1</v>
-      </c>
-      <c r="D10" s="12">
-        <v>2</v>
-      </c>
-      <c r="E10" s="12">
-        <v>3</v>
-      </c>
-      <c r="F10" s="12">
-        <v>4</v>
-      </c>
-      <c r="G10" s="12">
-        <v>5</v>
-      </c>
-      <c r="H10" s="12">
-        <v>6</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="E12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-    </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="B13" s="12"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>64</v>
-      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
-        <v>49</v>
+        <v>10</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0</v>
+      </c>
+      <c r="D19" s="12">
+        <v>1</v>
+      </c>
+      <c r="E19" s="12">
+        <v>2</v>
+      </c>
+      <c r="F19" s="12">
         <v>3</v>
       </c>
-      <c r="E19" s="5">
-        <v>10</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="G19" s="12">
+        <v>4</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="11" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="E26" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" s="12">
-        <v>0</v>
-      </c>
-      <c r="D34" s="12">
-        <v>1</v>
-      </c>
-      <c r="E34" s="12">
-        <v>2</v>
-      </c>
-      <c r="F34" s="12">
-        <v>3</v>
-      </c>
-      <c r="G34" s="12">
-        <v>4</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización del programa principal
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\TP final\TP final php\wordix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAAA709-310C-43A6-9D98-C82125AF33D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA274DA-9CF0-4A7A-A3D1-A9090EEFBD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,6 +395,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -459,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -503,6 +510,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:V1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1049,7 @@
         <v>7</v>
       </c>
       <c r="L15" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>8</v>
@@ -1077,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="5">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>8</v>
@@ -1096,7 +1106,7 @@
       <c r="P17" s="7"/>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L18" s="6"/>
+      <c r="L18" s="20"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>

</xml_diff>